<commit_message>
Get Trajectories by type and fileNameStartsWith from File System
</commit_message>
<xml_diff>
--- a/src/main/resources/INPUT/area/areas_BP23_A_ref.xlsx
+++ b/src/main/resources/INPUT/area/areas_BP23_A_ref.xlsx
@@ -338,7 +338,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -747,7 +747,7 @@
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D16" s="4" t="n">
         <v>400</v>

</xml_diff>